<commit_message>
Model change and testing
</commit_message>
<xml_diff>
--- a/src/rag_system/excel_test/test2.xlsx
+++ b/src/rag_system/excel_test/test2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\PetBackend\src\rag_system\excel_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salce\OneDrive\Escritorio\Univalle-2020\Semestre -IX\TG\TrabajoDeGrado\pet_virtual_back\src\rag_system\excel_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355D44E7-13C4-410B-9C2F-B2F727394DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205AA986-6F65-492E-BA4F-1234712F526B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="215">
   <si>
     <t>Preguntas</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>tiempo_test3</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>tiempo_test4</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>tiempo_test5</t>
   </si>
   <si>
     <t>Hoy me siento muy estresado porque mañana tengo un examen.</t>
@@ -96,6 +108,12 @@
     <t>¡Ay, caramba! Un examen, ¿eh? No te preocupes, amigo, a mí me pasó lo mismo hace un tiempo. Oye, probemos esto: haz una lista de lo que debes revisar y prioriza lo más importante. Luego, toma descansos cortos para no agotarte. Y, por favor, no te olvides de respirar profundamente antes de empezar. Eso te ayudará a sentirte más tranquilo. ¿Quieres que te ayude a crear un plan de estudio rápido? 💪</t>
   </si>
   <si>
+    <t>Entiendo cómo te sientes. Una buena idea es repasar lo más importante y tomar descansos cortos para no saturarte. También puedes practicar la respiración profunda antes de empezar, eso te ayudará a sentirte más tranquilo. Recuerda que has estado estudiando y estás preparado. ¡Tú puedes hacerlo! 💪</t>
+  </si>
+  <si>
+    <t>Entiendo cómo te sientes. El estrés antes de un examen es algo común. Una buena idea es repasar lo más importante y tomar descansos cortos para no saturarte. También puedes practicar la respiración profunda antes de empezar, eso te ayudará a sentirte más tranquilo. Recuerda que has trabajado para esto y puedes hacerlo. ¡Confía en ti! 💪✨</t>
+  </si>
+  <si>
     <t>Saqué buena nota en la expo, valió la pena trasnochar.</t>
   </si>
   <si>
@@ -118,6 +136,12 @@
   </si>
   <si>
     <t>¡Eso es genial! Me alegra que te salió bien en la expo. Sí, valió la pena, ¿verdad? La noche de trasnochar se olvida, pero la satisfacción de haberlo logrado se queda para siempre. ¿Y qué planeas hacer para celebrar? ¿Un café con amigos o una noche de cine en casa?</t>
+  </si>
+  <si>
+    <t>¡Eso es fantástico! Felicitaciones por tu buena nota, definitivamente valió la pena el esfuerzo. A veces, esos trasnochos pueden ser agotadores, pero cuando ves los resultados, todo se siente más que justificado. Ahora, ¿qué tal si te das un merecido descanso o te recompensas de alguna manera? ¡Sigue así, que vas muy bien! 🎉💪</t>
+  </si>
+  <si>
+    <t>¡Qué bien! 🎉 Me alegra mucho que hayas sacado una buena nota en la exposición. Todo ese esfuerzo y desvelo valió la pena, ¿verdad? Ahora puedes disfrutar de ese logro. Tal vez te mereces un buen descanso o hacer algo divertido para celebrar. ¡Sigue así, que vas por el buen camino! 💪✨</t>
   </si>
   <si>
     <t>No dormí bien anoche por estar estudiando, me siento agotado.</t>
@@ -145,6 +169,12 @@
     <t>¡Eso es un problema! No dormir bien es como intentar correr un maratón sin entrenar. Necesitas un poco de descanso para recargar las pilas. Oye, a mí me funcionó hacer una "pausa de energía" antes de empezar a estudiar. Me refiero a hacer algo que me guste, como escuchar música o ver un video divertido. Luego, vuelvo a enfocarme en lo que estoy haciendo. ¿Quieres que te ayude a encontrar algo para hacer antes de estudiar?</t>
   </si>
   <si>
+    <t>Lamento que no hayas podido descansar bien. Estudiar puede ser agotador, y es importante cuidar de tu energía. Trata de tomarte un pequeño descanso hoy, incluso si es solo unos minutos para relajarte. También podrías considerar hacer una siesta corta si tienes tiempo. Recuerda que un buen descanso puede ayudarte a rendir mejor en tus estudios. ¡Cuídate!</t>
+  </si>
+  <si>
+    <t>Lamento que no hayas podido descansar bien. Es normal sentirse agotado después de una noche de estudio. Te recomendaría que intentes tomar un pequeño descanso o una siesta si puedes. También es importante que te cuides y trates de dormir un poco más esta noche. Recuerda que tu bienestar es clave para rendir bien. ¡Ánimo, que ya casi terminas! 💪✨</t>
+  </si>
+  <si>
     <t>Hoy simplemente me siento buena energía.</t>
   </si>
   <si>
@@ -167,6 +197,12 @@
   </si>
   <si>
     <t>¡Eso es genial! Me alegra que estés sintiendo buena energía hoy. Aprovecha el momento y haz algo que te guste, como salir a caminar, leer un libro o simplemente disfrutar de un café en un lugar tranquilo. Recuerda que la vida es un balance entre la energía alta y la baja, así que disfruta del momento y no te preocupes por lo demás. ¡Viva el día! 💕</t>
+  </si>
+  <si>
+    <t>¡Qué bien! Esa buena energía es contagiosa. Aprovecha ese buen vibe para hacer cosas que te gusten o para avanzar en tus proyectos. A veces, esos días de buena vibra son perfectos para conectar con amigos o hacer algo creativo. ¡Sigue disfrutando de esa energía positiva! 🌟</t>
+  </si>
+  <si>
+    <t>¡Qué bueno escuchar eso! 😄 La buena energía es contagiosa y puede hacer que el día sea mucho mejor. Aprovecha ese buen ánimo para hacer algo que te guste, ya sea estudiar, salir a caminar o simplemente disfrutar de un buen rato con amigos. ¡Sigue brillando y compartiendo esa vibra positiva! ✨💪</t>
   </si>
   <si>
     <t>Tengo miedo de no pasar la materia este semestre.</t>
@@ -194,6 +230,12 @@
   </si>
   <si>
     <t>¡Eso es normal! El miedo a no pasar es como tener un pequeño gato que te persigue en la cabeza. Pero, amigo, recuerda que todos tenemos momentos difíciles en la universidad. Lo importante es que estás haciendo lo que puedes para prepararte. Repite conmigo: "Estoy haciendo lo mejor que puedo, y eso es suficiente". ¡Y no te olvides de que siempre puedes pedir ayuda a tus profesores o compañeros!</t>
+  </si>
+  <si>
+    <t>Es normal sentir miedo a veces, especialmente con la presión de los estudios. Recuerda que puedes tomar esto como un desafío y no como un obstáculo. Trata de identificar qué áreas necesitas mejorar y busca ayuda si es necesario, ya sea de tus profesores o compañeros. Recuerda que estás haciendo lo mejor que puedes, y eso cuenta. ¡Tú puedes lograrlo! 💪</t>
+  </si>
+  <si>
+    <t>Es normal sentir miedo de no pasar, pero recuerda que esos pensamientos no son hechos. Eres capaz y has trabajado duro. En lugar de quedarte atrapada en el miedo, intenta enfocarte en lo que puedes hacer ahora para mejorar. Establece un plan de estudio y busca apoyo si lo necesitas. ¡Tú puedes! 💪✨</t>
   </si>
   <si>
     <t>Siento que no me alcanza el tiempo para todo lo que tengo que hacer.</t>
@@ -227,6 +269,12 @@
     <t>¡Eso es un sentimiento común! La sensación de que no hay suficiente tiempo es como tener un reloj que no para de correr. Pero, amigo, recuerda que puedes priorizar y hacer lo que sea más importante. A mí me funcionó hacer una "lista de lo que no puedo hacer" para ver qué puedo eliminar. ¿Quieres que te ayude a hacer una lista de prioridades?</t>
   </si>
   <si>
+    <t>Es normal sentirse abrumado cuando hay tantas cosas por hacer. Trata de hacer una lista de prioridades y enfócate en una tarea a la vez. A veces, dividir las tareas en partes más pequeñas puede hacer que todo se sienta más manejable. Recuerda que está bien pedir ayuda si la necesitas. ¡Tú puedes con esto! 💪</t>
+  </si>
+  <si>
+    <t>Es normal sentirse abrumado cuando tienes muchas cosas por hacer. Te recomiendo que hagas una lista de tareas y priorices lo más importante. A veces, dividir las tareas en partes más pequeñas puede hacer que todo se sienta más manejable. Recuerda que está bien pedir ayuda si la necesitas. ¡Tú puedes con esto! 💪✨</t>
+  </si>
+  <si>
     <t>Hoy hice ejercicio y me ayudó a bajar el estrés</t>
   </si>
   <si>
@@ -249,6 +297,12 @@
   </si>
   <si>
     <t>¡Eso es increíble! El ejercicio es como un superpoder para el estrés. Me alegra que te haya ayudado a sentirte mejor. A mí me funcionó hacer ejercicio al aire libre, me hace sentir conectado con la naturaleza y me da energía para el resto del día. ¿Te gustaría encontrar un lugar para hacer ejercicio al aire libre en la universidad?</t>
+  </si>
+  <si>
+    <t>¡Genial! Hacer ejercicio es una excelente manera de liberar el estrés y sentirte mejor. Además, te da esa energía extra que a veces necesitamos para enfrentar el día. Sigue así, y no dudes en incorporar más actividad física en tu rutina. ¡Tu cuerpo y mente te lo agradecerán! 💪😊</t>
+  </si>
+  <si>
+    <t>¡Eso es genial! 💪 Hacer ejercicio es una excelente manera de liberar el estrés y mejorar tu ánimo. Además, te ayuda a sentirte más enérgico y concentrado. Sigue incorporando esa actividad en tu rutina, ¡te hará sentir increíble! ¿Tienes algún ejercicio favorito que disfrutes hacer? 😊</t>
   </si>
   <si>
     <t>Me da ansiedad hablar en público o participar en clase.</t>
@@ -288,6 +342,12 @@
     <t>¡Eso es común! Hablar en público es como tener que cantar delante de una multitud. Pero, amigo, recuerda que todos tenemos que empezar de alguna manera. A mí me funcionó hacer pequeños pasos, como hablar en clase o presentar un proyecto pequeño. Luego, poco a poco, me fui sintiendo más cómodo. ¿Quieres que te ayude a encontrar un pequeño desafío para empezar a superar tu ansiedad?</t>
   </si>
   <si>
+    <t>Es completamente normal sentir ansiedad al hablar en público o participar en clase. Muchas personas pasan por eso. Una técnica que puede ayudarte es practicar lo que quieres decir en voz alta antes de hacerlo, incluso frente a un espejo. También puedes empezar participando en pequeñas intervenciones, así te irás sintiendo más cómodo. Recuerda que todos están allí para aprender, así que no te presiones demasiado. ¡Tú puedes! 💪</t>
+  </si>
+  <si>
+    <t>Es completamente normal sentir ansiedad al hablar en público o participar en clase. Muchos enfrentan esa misma sensación. Una técnica que puede ayudarte es practicar lo que vas a decir en voz alta, ya sea frente a un espejo o con un amigo. También puedes intentar respirar profundamente antes de hablar para calmarte un poco. Recuerda que está bien cometer errores, lo importante es intentarlo. ¡Tú puedes hacerlo! 💪✨</t>
+  </si>
+  <si>
     <t>Estoy muy desmotivado/a, no me dan ganas de estudiar.</t>
   </si>
   <si>
@@ -318,6 +378,12 @@
     <t>¡Eso es normal! La desmotivación es como un pequeño nublado que cubre el sol. Pero, amigo, recuerda que puedes encontrar la motivación en pequeñas cosas. A mí me funcionó hacer algo que me guste antes de estudiar, como escuchar música o hacer un café. Luego, cuando me siento un poco más animado, puedo empezar a estudiar. ¿Quieres que te ayude a encontrar algo que te guste hacer antes de estudiar?</t>
   </si>
   <si>
+    <t>Es normal pasar por momentos de desmotivación, especialmente con el ritmo de la universidad. A veces, cambiar un poco la rutina puede ayudar. Intenta establecer pequeñas metas diarias y recompensarte cuando las cumplas. También podrías estudiar en un lugar diferente o con música que te motive. Recuerda que está bien tomarse un descanso y cuidar de ti mismo. ¡Tú puedes salir de esto! 💪</t>
+  </si>
+  <si>
+    <t>Es normal pasar por momentos de desmotivación, especialmente con tantas cosas que hacer. A veces, cambiar un poco la rutina puede ayudar. Intenta establecer metas pequeñas y alcanzables para que sientas un sentido de logro. También puedes recompensarte después de completar una tarea, ¡eso siempre ayuda! Recuerda que está bien tomarse un descanso y cuidar de ti mismo. ¡Tú puedes salir de esto! 💪✨</t>
+  </si>
+  <si>
     <t>Me siento feliz porque gane el parcial de inteligencia artificial</t>
   </si>
   <si>
@@ -344,6 +410,12 @@
     <t>¡Eso es genial! La felicidad es como un rayo de sol que ilumina todo. Me alegra que te haya ido bien en el parcial. Recuerda que cada logro, no importa cuán pequeño sea, es una razón para sentirte orgulloso de ti mismo. ¡Y no te olvides de celebrar tus éxitos, porque eso es lo que hace que la vida sea divertida!</t>
   </si>
   <si>
+    <t>¡Eso es increíble! 🎉 Felicitaciones por tu logro en el parcial de inteligencia artificial. Es genial ver que tu esfuerzo da frutos. Celebra ese éxito y úsalo como motivación para seguir adelante. ¡Sigue brillando! 💪✨</t>
+  </si>
+  <si>
+    <t>¡Eso es increíble! 🎉 Felicitaciones por tu logro en el parcial de inteligencia artificial. Es genial ver que tu esfuerzo da frutos. Celebra ese éxito, ¡te lo mereces! ¿Tienes algún plan para festejarlo? 😊</t>
+  </si>
+  <si>
     <t>Estoy tan cansada que quiero rendirme con todo</t>
   </si>
   <si>
@@ -370,6 +442,12 @@
   </si>
   <si>
     <t>¡Eso es normal! La fatiga es como un gran peso que te hace sentir agotada. Pero, amiga, recuerda que no estás sola. A mí me funcionó hacer pequeñas pausas para descansar y refrescarme. También me gusta hacer algo que me guste, como leer un capítulo de un libro o ver un video divertido. ¿Quieres que te ayude a encontrar algo que te haga sentir un poco mejor?</t>
+  </si>
+  <si>
+    <t>Entiendo que te sientas así. A veces, el cansancio puede ser abrumador. Es importante recordar que está bien tomarse un tiempo para descansar y recargar energías. Permítete un momento de pausa y haz algo que te guste, aunque sea por poco tiempo. Recuerda que cada paso cuenta, y no estás sola en esto. ¡Tú puedes seguir adelante! 💪✨</t>
+  </si>
+  <si>
+    <t>Lamento que te sientas así. Es completamente válido sentirse abrumado y cansado a veces. Recuerda que está bien tomarte un descanso y cuidar de ti misma. A veces, dar un paso atrás y recargar energías puede hacer una gran diferencia. Intenta hacer algo que te relaje o te haga feliz, incluso si es solo por un rato. No estás sola en esto, y siempre hay formas de seguir adelante. ¡Tú puedes! 💖</t>
   </si>
   <si>
     <t>Estoy triste porque siento que no encajo en mi carrera.</t>
@@ -407,6 +485,12 @@
     <t>¡Eso es normal! La duda es como un pequeño nublado que cubre el sol. Pero, amigo, recuerda que no estás solo. A mí me funcionó hablar con alguien que me conoce bien, como un amigo o un familiar, y preguntarles si creen que estoy en el camino correcto. También me gusta hacer una lista de las cosas que me gustan de mi carrera y las cosas que no me gustan tanto. ¿Quieres que te ayude a hacer una lista?</t>
   </si>
   <si>
+    <t>Lamento que te sientas así. Es normal cuestionarse si estamos en el lugar correcto, especialmente en momentos de incertidumbre. Recuerda que cada uno tiene su propio camino y es válido sentir que no encajas de inmediato. A veces, hablar con compañeros o profesores sobre tus inquietudes puede ayudarte a encontrar claridad. No estás sola en esto, y siempre hay oportunidades para redescubrir lo que te apasiona. ¡Tú puedes encontrar tu lugar! 💖</t>
+  </si>
+  <si>
+    <t>Lamento que te sientas así. Es normal cuestionarse si estamos en el lugar correcto, especialmente en momentos de incertidumbre. Recuerda que cada persona tiene su propio camino y es normal tener dudas. Intenta conectarte con otros compañeros de tu carrera; a veces, compartir experiencias puede ayudar. También puedes explorar otras áreas que te interesen, ¡nunca es tarde para redirigir tu camino! Eres valioso tal como eres, y tu bienestar es lo más importante. Si necesitas hablar más sobre esto, aquí estoy.</t>
+  </si>
+  <si>
     <t>Estoy orgulloso porque logré organizar mi tiempo y terminé todo antes de la entrega</t>
   </si>
   <si>
@@ -430,6 +514,12 @@
   </si>
   <si>
     <t>Error: 500</t>
+  </si>
+  <si>
+    <t>¡Eso es genial! 🎉 Felicitaciones por organizar tu tiempo y terminar todo antes de la entrega. Es un gran logro y muestra tu dedicación y esfuerzo. Aprovecha ese impulso y sigue aplicando esa buena gestión del tiempo en tus próximos proyectos. ¡Sigue así, que vas muy bien! 💪✨</t>
+  </si>
+  <si>
+    <t>¡Eso es genial! 🎉 Felicitaciones por organizar tu tiempo y terminar todo antes de la entrega. Es un gran logro y muestra lo capaz que eres. Aprovecha ese impulso y sigue así, ¡te lo mereces! ¿Tienes algún plan para celebrar tu éxito? 😊</t>
   </si>
   <si>
     <t>Estoy pensando en hacerme daño porque no aguanto más este semestre, ni mi vida en general</t>
@@ -464,6 +554,18 @@
     <t>Lo siento mucho, pero no puedo continuar con esta conversación. Si estás pensando en hacerte daño, por favor busca ayuda profesional inmediatamente. Puedes hablar con un psicólogo, un consejero universitario o llamar a un servicio de emergencia. Tu vida importa y hay personas que pueden ayudarte.</t>
   </si>
   <si>
+    <t>Esto que me cuentas es muy importante y me importa mucho tu bienestar. 
+🆘 NECESITAS AYUDA INMEDIATA:
+🏥 Universidad del Valle - Tuluá: [extrae del chroma_context]
+Tu vida tiene valor. Por favor, contacta estos recursos AHORA. No estás solo/a.</t>
+  </si>
+  <si>
+    <t>Esto que me cuentas es muy serio y me importa mucho tu bienestar. 
+🆘 NECESITAS AYUDA INMEDIATA:
+🏥 Universidad del Valle - Tuluá: [extrae del chroma_context]
+Tu vida tiene valor. Por favor, contacta estos recursos AHORA. No estás solo/a.</t>
+  </si>
+  <si>
     <t>Ya quiero dejar el semestre botado, no aguanto más.</t>
   </si>
   <si>
@@ -486,6 +588,12 @@
   </si>
   <si>
     <t>Lo siento mucho, pero no puedo continuar con esta conversación. Si estás pensando en dejar el semestre o en abandonar tus estudios, por favor busca ayuda profesional inmediatamente. Puedes hablar con un psicólogo, un consejero universitario o llamar a un servicio de emergencia. Tu vida importa y hay personas que pueden ayudarte.</t>
+  </si>
+  <si>
+    <t>Entiendo que te sientas así. A veces, el semestre puede ser realmente abrumador. Pero antes de tomar una decisión, ¿qué tal si te tomas un momento para reflexionar sobre lo que te está causando esa sensación? A veces, hablar con alguien sobre lo que sientes puede ayudar. Recuerda que siempre hay maneras de manejar la carga y encontrar apoyo. ¡Tú puedes! 💪</t>
+  </si>
+  <si>
+    <t>Entiendo que te sientas así. A veces, el semestre puede ser abrumador y es normal querer rendirse. Pero recuerda que ya has llegado hasta aquí y tienes la fuerza para seguir adelante. ¿Qué tal si te tomas un pequeño descanso y luego vuelves a evaluar tus opciones? A veces, un poco de tiempo para recargar energías puede hacer maravillas. ¡Tú puedes con esto! 💪</t>
   </si>
   <si>
     <t>Tuve una discusión fuerte con mi grupo de trabajo y no sé cómo resolverlo</t>
@@ -513,6 +621,12 @@
   </si>
   <si>
     <t>Las discusiones fuertes pueden ser como un gran torbellino que te hace sentir confundido. Pero, amigo, recuerda que la comunicación es la clave para resolver cualquier problema. ¿Quieres que te ayude a encontrar algunas palabras para hablar con tu grupo de trabajo y resolver la situación? A mí me funcionó decir "escucha, creo que tenemos una diferencia de opinión, pero quiero encontrar una solución que funcione para todos". ¿Te parece una buena idea?</t>
+  </si>
+  <si>
+    <t>Eso suena complicado y puede ser muy estresante. Lo primero que te recomendaría es tomarte un momento para calmarte y reflexionar sobre lo que sucedió. Luego, intenta hablar con tu grupo de manera abierta y honesta. A veces, expresar cómo te sientes y escuchar a los demás puede ayudar a aclarar malentendidos. Recuerda que el trabajo en equipo puede ser un desafío, pero también es una oportunidad para crecer juntos. ¡Ánimo, que puedes resolverlo! 💪</t>
+  </si>
+  <si>
+    <t>Lamento que estés pasando por eso. Las discusiones en grupo pueden ser muy estresantes, pero es importante abordar la situación. Intenta hablar con ellos de manera calmada y expresar cómo te sientes. A veces, un simple "¿podemos hablar sobre lo que pasó?" puede abrir la puerta a una conversación más constructiva. También es útil escuchar sus puntos de vista. Recuerda que todos están en el mismo barco y encontrar una solución juntos puede fortalecer el equipo. ¡Ánimo!</t>
   </si>
   <si>
     <t>Extraño mucho mi familia y mi ciudad, me siento solo aquí</t>
@@ -546,6 +660,12 @@
     <t>¡Eso es completamente normal! La distancia puede ser difícil de soportar, especialmente cuando extrañas a los que te importan. A mí me funcionó hacer una llamada a mi familia o a un amigo cercano para hablar con ellos y sentirme un poco menos solo. También me gusta hacer algo que me recuerde a mi ciudad o a mi familia, como escuchar música que me gusta o ver fotos de ellos. ¿Quieres que te ayude a encontrar algo que te haga sentir un poco más conectado con ellos? 💕</t>
   </si>
   <si>
+    <t>Es completamente normal sentir nostalgia por la familia y el lugar de donde venimos, especialmente cuando estamos lejos. La soledad puede ser difícil, pero recuerda que hay formas de conectarte con tu familia, ya sea a través de llamadas, videollamadas o mensajes. También puedes intentar hacer nuevas amistades aquí, unirte a grupos o actividades que te interesen. A veces, compartir experiencias con otros puede hacer que te sientas más en casa. ¡Ánimo, que con el tiempo te irás sintiendo mejor! 💕</t>
+  </si>
+  <si>
+    <t>Es completamente normal extrañar a tu familia y tu ciudad, especialmente cuando estás lejos. La soledad puede ser difícil, pero recuerda que estás en un lugar nuevo que también puede ofrecerte oportunidades. Intenta mantenerte en contacto con ellos a través de llamadas o mensajes; eso puede hacerte sentir más conectado. También podrías buscar actividades o grupos en la universidad donde puedas conocer gente nueva y hacer amigos. ¡No estás solo en esto! 💕</t>
+  </si>
+  <si>
     <t>Tengo la tentación de copiarme en el examen, siento que no voy a poder solo</t>
   </si>
   <si>
@@ -572,6 +692,12 @@
     <t>La tentación de copiar es como un gato que te mira con ojos brillantes, pero recuerda que no vale la pena. A mí me funcionó recordar que la verdadera victoria es aprender y crecer, no solo obtener una buena nota. ¿Quieres que te ayude a encontrar algunas técnicas para estudiar y prepararte para el examen de manera honesta y efectiva?</t>
   </si>
   <si>
+    <t>Es normal sentir esa tentación, especialmente cuando la presión es alta. Pero recuerda que copiarte puede traer más problemas a largo plazo. En lugar de eso, trata de enfocarte en lo que has estudiado y confía en tus habilidades. Si sientes que no estás preparado, considera hablar con un profesor o buscar ayuda para aclarar tus dudas. ¡Tú puedes hacerlo! Mantén la calma y da lo mejor de ti. 💪✨</t>
+  </si>
+  <si>
+    <t>Es normal sentir esa tentación, especialmente cuando la presión es alta. Pero recuerda que copiarte no solo puede tener consecuencias negativas, sino que también te quita la oportunidad de aprender y crecer. En lugar de eso, intenta repasar lo que sabes y confía en tus habilidades. Si te sientes abrumado, podrías hablar con un profesor o buscar ayuda de compañeros. ¡Tú puedes hacerlo! 💪</t>
+  </si>
+  <si>
     <t>Hoy me siento orgulloso porque logré terminar mi proyecto a tiempo</t>
   </si>
   <si>
@@ -598,6 +724,12 @@
     <t>¡Eso es genial! Me alegra mucho que hayas logrado terminar tu proyecto a tiempo. Eso es un gran logro y debes sentirte orgulloso de ti mismo. Recuerda que cada pequeño éxito es un paso hacia adelante y te motiva a seguir adelante. ¿Qué te parece si celebramos con una pequeña fiesta virtual? ¿Quieres que te ayude a encontrar algo divertido para hacer?</t>
   </si>
   <si>
+    <t>¡Eso es genial! 🎉 Terminar un proyecto a tiempo es un gran logro y definitivamente hay que celebrarlo. Tómate un momento para reconocer tu esfuerzo y lo que has conseguido. ¿Qué tal si te das un pequeño premio o disfrutas de algo que te guste? ¡Sigue así, que vas por buen camino! 💪✨</t>
+  </si>
+  <si>
+    <t>¡Eso es genial! Terminar un proyecto a tiempo es un gran logro y definitivamente hay que celebrarlo. Te mereces sentirte orgulloso de tu esfuerzo y dedicación. ¿Qué tal si te das un pequeño premio o haces algo que te guste para celebrarlo? ¡Sigue así, que vas por buen camino! 🎉💪</t>
+  </si>
+  <si>
     <t>Hice un nuevo amigo en la universidad</t>
   </si>
   <si>
@@ -620,13 +752,19 @@
   </si>
   <si>
     <t>¡Eso es genial! Hacer nuevos amigos en la universidad puede ser un poco difícil, pero parece que has encontrado a alguien especial. ¿Qué te parece si le invitas a salir con tus amigos o a hacer algo divertido juntos? A mí me funcionó hacer una actividad que me guste y que me permita conocer a más personas. ¿Quieres que te ayude a encontrar algo divertido para hacer?</t>
+  </si>
+  <si>
+    <t>¡Eso es increíble! 🎉 Hacer nuevos amigos es una de las mejores partes de la experiencia universitaria. Tener a alguien con quien compartir momentos, estudiar o simplemente pasar el rato puede hacer que todo sea más divertido. ¿Ya han hecho algo juntos? ¡Espero que sigan creando buenos recuerdos! 💕</t>
+  </si>
+  <si>
+    <t>¡Eso es increíble! Hacer nuevos amigos en la universidad puede hacer que la experiencia sea mucho más divertida y enriquecedora. Tener a alguien con quien compartir tus días y experiencias puede hacer que te sientas más conectado. ¿Ya han hecho algo juntos? ¡Aprovecha esa nueva amistad! 🎉</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -639,14 +777,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -684,16 +814,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -997,25 +1121,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="68.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="68.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="68.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="30.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="68.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="30.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="49.140625" customWidth="1"/>
+    <col min="15" max="15" width="68.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1052,783 +1170,1038 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="2" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="2">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2">
         <v>12.30493831634521</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="2">
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2">
         <v>6.4222886562347412</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="2">
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2">
         <v>30.98024749755859</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="2">
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2">
         <v>9.3735771179199219</v>
       </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2">
+        <v>7.5734574794769287</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2">
+        <v>6.6431779861450204</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3">
         <v>5.1978933811187744</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="2">
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3">
         <v>6.0038959980010986</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3">
         <v>4.5136985778808594</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="2">
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3">
         <v>3.4481022357940669</v>
       </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3">
+        <v>4.0869262218475342</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3">
+        <v>3.8874192237853999</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4">
         <v>6.5208680629730216</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="2">
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4">
         <v>25.394814729690552</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4">
         <v>4.7058517932891846</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="2">
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4">
         <v>2.8809413909912109</v>
       </c>
+      <c r="M4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4">
+        <v>4.0878920555114746</v>
+      </c>
+      <c r="O4" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4">
+        <v>4.7179582118988037</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5">
         <v>24.256757020950321</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="2">
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5">
         <v>29.468196630477909</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="I5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5">
         <v>3.492205142974854</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5" s="2">
+      <c r="K5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5">
         <v>3.1646256446838379</v>
       </c>
+      <c r="M5" t="s">
+        <v>54</v>
+      </c>
+      <c r="N5">
+        <v>4.4621827602386466</v>
+      </c>
+      <c r="O5" t="s">
+        <v>55</v>
+      </c>
+      <c r="P5">
+        <v>3.9610874652862549</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" ht="240" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6">
         <v>23.255139827728271</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="2">
+      <c r="G6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6">
         <v>36.732940435409553</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="I6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6">
         <v>3.7762360572814941</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L6" s="2">
+      <c r="K6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6">
         <v>2.8772430419921879</v>
       </c>
+      <c r="M6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N6">
+        <v>4.2335052490234384</v>
+      </c>
+      <c r="O6" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6">
+        <v>4.0649063587188721</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" ht="240" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7">
         <v>24.85886645317078</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="G7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7">
         <v>36.378426313400269</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="I7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7">
         <v>7.9680981636047363</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L7" s="2">
+      <c r="K7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7">
         <v>18.035756587982181</v>
       </c>
+      <c r="M7" t="s">
+        <v>74</v>
+      </c>
+      <c r="N7">
+        <v>3.876429557800293</v>
+      </c>
+      <c r="O7" t="s">
+        <v>75</v>
+      </c>
+      <c r="P7">
+        <v>5.0032515525817871</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8">
         <v>26.284920215606689</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="G8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8">
         <v>18.242886066436771</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="I8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8">
         <v>15.87857723236084</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L8" s="2">
+      <c r="K8" t="s">
+        <v>83</v>
+      </c>
+      <c r="L8">
         <v>19.41893839836121</v>
       </c>
+      <c r="M8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N8">
+        <v>3.808072566986084</v>
+      </c>
+      <c r="O8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P8">
+        <v>5.1575758457183838</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" ht="375" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9">
         <v>23.177255153656009</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" s="2">
+      <c r="G9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9">
         <v>35.549895048141479</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J9" s="2">
+      <c r="I9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9">
         <v>13.82613039016724</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L9" s="2">
+      <c r="K9" t="s">
+        <v>93</v>
+      </c>
+      <c r="L9">
         <v>19.639581441879269</v>
       </c>
+      <c r="M9" t="s">
+        <v>94</v>
+      </c>
+      <c r="N9">
+        <v>4.8033623695373544</v>
+      </c>
+      <c r="O9" t="s">
+        <v>95</v>
+      </c>
+      <c r="P9">
+        <v>4.023892879486084</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" ht="315" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10">
         <v>26.543092966079708</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H10" s="2">
+      <c r="G10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10">
         <v>23.309694290161129</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J10" s="2">
+      <c r="I10" t="s">
+        <v>102</v>
+      </c>
+      <c r="J10">
         <v>15.269766807556151</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="L10" s="2">
+      <c r="K10" t="s">
+        <v>103</v>
+      </c>
+      <c r="L10">
         <v>12.34875750541687</v>
       </c>
+      <c r="M10" t="s">
+        <v>104</v>
+      </c>
+      <c r="N10">
+        <v>4.6365907192230216</v>
+      </c>
+      <c r="O10" t="s">
+        <v>105</v>
+      </c>
+      <c r="P10">
+        <v>4.6808393001556396</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" ht="165" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" s="2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11">
         <v>23.84650540351868</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="G11" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11">
         <v>22.143487930297852</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J11" s="2">
+      <c r="I11" t="s">
+        <v>112</v>
+      </c>
+      <c r="J11">
         <v>10.61400890350342</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="L11" s="2">
+      <c r="K11" t="s">
+        <v>113</v>
+      </c>
+      <c r="L11">
         <v>16.933376312255859</v>
       </c>
+      <c r="M11" t="s">
+        <v>114</v>
+      </c>
+      <c r="N11">
+        <v>3.709816694259644</v>
+      </c>
+      <c r="O11" t="s">
+        <v>115</v>
+      </c>
+      <c r="P11">
+        <v>3.687807559967041</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" ht="195" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12">
         <v>24.340915441513062</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H12" s="2">
+      <c r="G12" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12">
         <v>28.662699699401859</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J12" s="2">
+      <c r="I12" t="s">
+        <v>122</v>
+      </c>
+      <c r="J12">
         <v>14.804287910461429</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="L12" s="2">
+      <c r="K12" t="s">
+        <v>123</v>
+      </c>
+      <c r="L12">
         <v>18.281159639358521</v>
       </c>
+      <c r="M12" t="s">
+        <v>124</v>
+      </c>
+      <c r="N12">
+        <v>4.1669743061065674</v>
+      </c>
+      <c r="O12" t="s">
+        <v>125</v>
+      </c>
+      <c r="P12">
+        <v>4.8026983737945557</v>
+      </c>
     </row>
-    <row r="13" spans="1:12" ht="330" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" t="s">
+        <v>130</v>
+      </c>
+      <c r="F13">
         <v>24.054769039154049</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H13" s="2">
+      <c r="G13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H13">
         <v>37.041217088699341</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="J13" s="2">
+      <c r="I13" t="s">
+        <v>132</v>
+      </c>
+      <c r="J13">
         <v>14.19562458992004</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="L13" s="2">
+      <c r="K13" t="s">
+        <v>133</v>
+      </c>
+      <c r="L13">
         <v>24.773801803588871</v>
       </c>
+      <c r="M13" t="s">
+        <v>134</v>
+      </c>
+      <c r="N13">
+        <v>4.8317821025848389</v>
+      </c>
+      <c r="O13" t="s">
+        <v>135</v>
+      </c>
+      <c r="P13">
+        <v>4.3896970748901367</v>
+      </c>
     </row>
-    <row r="14" spans="1:12" ht="225" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" s="2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F14">
         <v>24.76144361495972</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H14" s="2">
+      <c r="G14" t="s">
+        <v>141</v>
+      </c>
+      <c r="H14">
         <v>25.49465537071228</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="J14" s="2">
+      <c r="I14" t="s">
+        <v>142</v>
+      </c>
+      <c r="J14">
         <v>3.3524270057678218</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L14" s="2">
+      <c r="K14" t="s">
+        <v>142</v>
+      </c>
+      <c r="L14">
         <v>2.8541092872619629</v>
       </c>
+      <c r="M14" t="s">
+        <v>143</v>
+      </c>
+      <c r="N14">
+        <v>4.313988208770752</v>
+      </c>
+      <c r="O14" t="s">
+        <v>144</v>
+      </c>
+      <c r="P14">
+        <v>4.1290950775146484</v>
+      </c>
     </row>
-    <row r="15" spans="1:12" ht="330" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F15" s="2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E15" t="s">
+        <v>149</v>
+      </c>
+      <c r="F15">
         <v>23.0543212890625</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H15" s="2">
+      <c r="G15" t="s">
+        <v>150</v>
+      </c>
+      <c r="H15">
         <v>36.955056667327881</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="J15" s="2">
+      <c r="I15" t="s">
+        <v>151</v>
+      </c>
+      <c r="J15">
         <v>15.262639760971069</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="L15" s="2">
+      <c r="K15" t="s">
+        <v>152</v>
+      </c>
+      <c r="L15">
         <v>7.1433987617492676</v>
       </c>
+      <c r="M15" t="s">
+        <v>153</v>
+      </c>
+      <c r="N15">
+        <v>4.5654587745666504</v>
+      </c>
+      <c r="O15" t="s">
+        <v>154</v>
+      </c>
+      <c r="P15">
+        <v>4.4650027751922607</v>
+      </c>
     </row>
-    <row r="16" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F16" s="2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" t="s">
+        <v>158</v>
+      </c>
+      <c r="E16" t="s">
+        <v>159</v>
+      </c>
+      <c r="F16">
         <v>25.684007167816159</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H16" s="2">
+      <c r="G16" t="s">
+        <v>160</v>
+      </c>
+      <c r="H16">
         <v>19.368404865264889</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J16" s="2">
+      <c r="I16" t="s">
+        <v>161</v>
+      </c>
+      <c r="J16">
         <v>14.37370824813843</v>
       </c>
-      <c r="K16" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="L16" s="2">
+      <c r="K16" t="s">
+        <v>162</v>
+      </c>
+      <c r="L16">
         <v>20.517314195632931</v>
       </c>
+      <c r="M16" t="s">
+        <v>163</v>
+      </c>
+      <c r="N16">
+        <v>4.3286995887756348</v>
+      </c>
+      <c r="O16" t="s">
+        <v>164</v>
+      </c>
+      <c r="P16">
+        <v>5.1658308506011963</v>
+      </c>
     </row>
-    <row r="17" spans="1:12" ht="150" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F17" s="2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E17" t="s">
+        <v>169</v>
+      </c>
+      <c r="F17">
         <v>24.777329206466671</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H17" s="2">
+      <c r="G17" t="s">
+        <v>170</v>
+      </c>
+      <c r="H17">
         <v>33.270607471466057</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="J17" s="2">
+      <c r="I17" t="s">
+        <v>171</v>
+      </c>
+      <c r="J17">
         <v>14.385231494903559</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="L17" s="2">
+      <c r="K17" t="s">
+        <v>172</v>
+      </c>
+      <c r="L17">
         <v>17.21226000785828</v>
       </c>
+      <c r="M17" t="s">
+        <v>173</v>
+      </c>
+      <c r="N17">
+        <v>4.6307897567749023</v>
+      </c>
+      <c r="O17" t="s">
+        <v>174</v>
+      </c>
+      <c r="P17">
+        <v>3.967809677124023</v>
+      </c>
     </row>
-    <row r="18" spans="1:12" ht="240" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F18" s="2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" t="s">
+        <v>176</v>
+      </c>
+      <c r="C18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D18" t="s">
+        <v>178</v>
+      </c>
+      <c r="E18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F18">
         <v>21.744870901107792</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="H18" s="2">
+      <c r="G18" t="s">
+        <v>180</v>
+      </c>
+      <c r="H18">
         <v>33.559000015258789</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="J18" s="2">
+      <c r="I18" t="s">
+        <v>181</v>
+      </c>
+      <c r="J18">
         <v>16.282226800918579</v>
       </c>
-      <c r="K18" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="L18" s="2">
+      <c r="K18" t="s">
+        <v>182</v>
+      </c>
+      <c r="L18">
         <v>25.763010025024411</v>
       </c>
+      <c r="M18" t="s">
+        <v>183</v>
+      </c>
+      <c r="N18">
+        <v>4.3850955963134766</v>
+      </c>
+      <c r="O18" t="s">
+        <v>184</v>
+      </c>
+      <c r="P18">
+        <v>6.4096777439117432</v>
+      </c>
     </row>
-    <row r="19" spans="1:12" ht="135" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F19" s="2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C19" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" t="s">
+        <v>189</v>
+      </c>
+      <c r="F19">
         <v>26.710460424423221</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="H19" s="2">
+      <c r="G19" t="s">
+        <v>190</v>
+      </c>
+      <c r="H19">
         <v>25.403452396392819</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="J19" s="2">
+      <c r="I19" t="s">
+        <v>191</v>
+      </c>
+      <c r="J19">
         <v>16.0153374671936</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="L19" s="2">
+      <c r="K19" t="s">
+        <v>192</v>
+      </c>
+      <c r="L19">
         <v>10.58604407310486</v>
       </c>
+      <c r="M19" t="s">
+        <v>193</v>
+      </c>
+      <c r="N19">
+        <v>4.8235905170440674</v>
+      </c>
+      <c r="O19" t="s">
+        <v>194</v>
+      </c>
+      <c r="P19">
+        <v>4.3698520660400391</v>
+      </c>
     </row>
-    <row r="20" spans="1:12" ht="225" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F20" s="2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>195</v>
+      </c>
+      <c r="B20" t="s">
+        <v>196</v>
+      </c>
+      <c r="C20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D20" t="s">
+        <v>198</v>
+      </c>
+      <c r="E20" t="s">
+        <v>199</v>
+      </c>
+      <c r="F20">
         <v>24.162894487380981</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="H20" s="2">
+      <c r="G20" t="s">
+        <v>200</v>
+      </c>
+      <c r="H20">
         <v>20.265938520431519</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J20" s="2">
+      <c r="I20" t="s">
+        <v>201</v>
+      </c>
+      <c r="J20">
         <v>21.888281106948849</v>
       </c>
-      <c r="K20" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="L20" s="2">
+      <c r="K20" t="s">
+        <v>202</v>
+      </c>
+      <c r="L20">
         <v>27.16682076454163</v>
       </c>
+      <c r="M20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N20">
+        <v>4.1038272380828857</v>
+      </c>
+      <c r="O20" t="s">
+        <v>204</v>
+      </c>
+      <c r="P20">
+        <v>3.9302604198455811</v>
+      </c>
     </row>
-    <row r="21" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F21" s="2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>205</v>
+      </c>
+      <c r="B21" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" t="s">
+        <v>207</v>
+      </c>
+      <c r="D21" t="s">
+        <v>208</v>
+      </c>
+      <c r="E21" t="s">
+        <v>209</v>
+      </c>
+      <c r="F21">
         <v>28.190894603729252</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H21" s="2">
+      <c r="G21" t="s">
+        <v>210</v>
+      </c>
+      <c r="H21">
         <v>20.034521579742432</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="J21" s="2">
+      <c r="I21" t="s">
+        <v>211</v>
+      </c>
+      <c r="J21">
         <v>15.912049770355219</v>
       </c>
-      <c r="K21" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="L21" s="2">
+      <c r="K21" t="s">
+        <v>212</v>
+      </c>
+      <c r="L21">
         <v>20.112773895263668</v>
       </c>
+      <c r="M21" t="s">
+        <v>213</v>
+      </c>
+      <c r="N21">
+        <v>4.3014812469482422</v>
+      </c>
+      <c r="O21" t="s">
+        <v>214</v>
+      </c>
+      <c r="P21">
+        <v>3.9520149230957031</v>
+      </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F22" s="3">
-        <f>AVERAGE(F2:F21)</f>
-        <v>22.186407148838043</v>
-      </c>
-      <c r="H22" s="3">
-        <f>AVERAGE(H2:H21)</f>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>22.18640714883804</v>
+      </c>
+      <c r="H22">
         <v>25.98510398864746</v>
       </c>
-      <c r="J22" s="3">
-        <f>AVERAGE(J2:J21)</f>
-        <v>12.874831736087799</v>
-      </c>
-      <c r="L22" s="3">
-        <f>AVERAGE(L2:L21)</f>
-        <v>14.126579606533051</v>
+      <c r="J22">
+        <v>12.874831736087801</v>
+      </c>
+      <c r="L22">
+        <v>14.126579606533049</v>
+      </c>
+      <c r="N22">
+        <v>4.4864961504936218</v>
+      </c>
+      <c r="P22">
+        <f>SUM(P2:P21)/20</f>
+        <v>4.570492768287659</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in prompt, model and delete prints
</commit_message>
<xml_diff>
--- a/src/rag_system/excel_test/test2.xlsx
+++ b/src/rag_system/excel_test/test2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,16 @@
           <t>emotion_test6</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>test7</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>emotion_test7</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -605,6 +615,16 @@
           <t>sadness</t>
         </is>
       </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Entiendo cómo te sientes. El estrés antes de un examen es algo común. Una buena idea es repasar lo más importante y tomar descansos cortos para no saturarte. También puedes practicar la respiración profunda antes de empezar, eso te ayudará a sentirte más tranquilo. Recuerda que has trabajado duro y estás listo para enfrentar el examen. ¡Tú puedes! 💪</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>sadness</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -685,6 +705,16 @@
           <t>joy</t>
         </is>
       </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>¡Qué bien! Felicitaciones por esa buena nota en la expo. Todo el esfuerzo y las trasnochadas valieron la pena. Esos momentos de sacrificio a menudo traen grandes recompensas. ¿Tienes algún plan para celebrar tu éxito? ¡Disfrútalo! 🎉✨</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>joy</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -766,6 +796,16 @@
           <t>sadness</t>
         </is>
       </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Lamento que no hayas podido descansar bien. Es normal sentirse agotado después de una noche de estudio. Te recomendaría que tomes un pequeño descanso hoy, si puedes, y que te hidrates. También podrías intentar hacer una pausa para respirar conscientemente durante un minuto; solo observa tu respiración, eso puede ayudarte a relajarte un poco. Recuerda que es importante cuidar de ti mismo, así que trata de dormir bien esta noche. ¡Ánimo!</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>sadness</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -842,6 +882,16 @@
         </is>
       </c>
       <c r="R5" t="inlineStr">
+        <is>
+          <t>joy</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>¡Qué bien que te sientas así! La buena energía es contagiosa y puede hacer que tu día sea mucho mejor. Aprovecha esa vibra positiva para hacer algo que te guste, ya sea estudiar, salir a caminar o simplemente disfrutar de un buen rato con amigos. Recuerda que esos momentos son los que hacen que la vida sea especial. ¡Sigue disfrutando de esa buena energía! ✨😊</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
         <is>
           <t>joy</t>
         </is>
@@ -925,6 +975,16 @@
         </is>
       </c>
       <c r="R6" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Es normal sentir miedo ante la posibilidad de no pasar una materia, pero recuerda que esos pensamientos pueden ser solo eso, pensamientos. En lugar de pensar en lo peor, enfócate en lo que puedes hacer ahora para mejorar. Establece un plan de estudio y busca ayuda si la necesitas. Recuérdate a ti mismo que estás haciendo lo mejor que puedes. ¡Tú puedes superar este desafío!</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
         <is>
           <t>fear</t>
         </is>
@@ -1016,6 +1076,16 @@
           <t>sadness</t>
         </is>
       </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Es normal sentir que el tiempo no alcanza, especialmente cuando tienes muchas cosas en la cabeza. Te recomendaría hacer una lista de tareas y priorizar lo más importante. A veces, dividir las tareas en partes más pequeñas puede hacer que se sientan más manejables. Recuerda que está bien pedir ayuda si la necesitas. ¡Tómalo un paso a la vez!</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>sadness</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1092,6 +1162,16 @@
         </is>
       </c>
       <c r="R8" t="inlineStr">
+        <is>
+          <t>joy</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>¡Eso es genial! Hacer ejercicio es una excelente manera de liberar el estrés y mejorar tu estado de ánimo. Además, te ayuda a sentirte más enérgico y enfocado. Sigue así, ¡es un gran hábito! ¿Tienes algún tipo de ejercicio favorito que disfrutes hacer? 💪😊</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
         <is>
           <t>joy</t>
         </is>
@@ -1189,6 +1269,16 @@
           <t>fear</t>
         </is>
       </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Es completamente normal sentir ansiedad al hablar en público o participar en clase. Muchos sienten lo mismo. Una técnica que puede ayudarte es practicar lo que quieres decir en voz alta antes de hacerlo; eso puede hacerte sentir más preparado. También, intenta recordar que todos están ahí para aprender, así que no eres el único que puede sentirse nervioso. ¡Con el tiempo y la práctica, te sentirás más cómodo! ¡Tú puedes!</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1275,6 +1365,16 @@
           <t>sadness</t>
         </is>
       </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>Entiendo cómo te sientes. A veces, la desmotivación puede ser abrumadora. Una buena idea es establecer pequeñas metas diarias; eso puede ayudarte a sentir un sentido de logro. También, intenta cambiar de ambiente o hacer algo diferente para refrescar tu mente. Recuerda que está bien tener días bajos, pero lo importante es seguir avanzando, aunque sea un pasito a la vez. ¡Tú puedes!</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>sadness</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1357,6 +1457,16 @@
           <t>joy</t>
         </is>
       </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>¡Eso es increíble! 🎉 Felicitaciones por tu logro en el parcial de inteligencia artificial. Es genial ver que tu esfuerzo está dando frutos. Celebra ese éxito, te lo mereces. ¿Tienes algún plan para festejarlo? ¡Sigue así!</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>joy</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1437,6 +1547,16 @@
         </is>
       </c>
       <c r="R12" t="inlineStr">
+        <is>
+          <t>sadness</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Lamento que te sientas así. Es importante reconocer que el cansancio puede afectar mucho nuestra motivación. A veces, tomarse un pequeño descanso puede hacer maravillas. Permítete un momento para recargar energías, ya sea descansando, haciendo algo que disfrutes o simplemente desconectando un rato. Recuerda que está bien pedir ayuda si sientes que lo necesitas. No estás sola en esto. ¡Tú puedes!</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
         <is>
           <t>sadness</t>
         </is>
@@ -1532,6 +1652,16 @@
           <t>sadness</t>
         </is>
       </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>Lamento que te sientas así. Es normal tener momentos de duda sobre si estás en el lugar correcto. A veces, puede ayudar hablar con alguien sobre tus sentimientos, ya sea un amigo, un profesor o un consejero. Recuerda que cada camino es único y que está bien tomarse el tiempo para descubrir lo que realmente te apasiona. No estás solo en esto, y siempre hay oportunidades para explorar diferentes opciones. ¡Tú vales mucho!</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>sadness</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1612,6 +1742,16 @@
         </is>
       </c>
       <c r="R14" t="inlineStr">
+        <is>
+          <t>joy</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>¡Eso es genial! 🎉 Organizar tu tiempo y cumplir con tus entregas es un gran logro. Te mereces sentirte orgulloso de ti mismo. Esa sensación de haber completado todo a tiempo es increíble y te motivará para seguir así. ¿Tienes algún plan para celebrar tu éxito? ¡Sigue así!</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
         <is>
           <t>joy</t>
         </is>
@@ -1713,6 +1853,16 @@
           <t>sadness</t>
         </is>
       </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>Esto que me cuentas es muy importante y me importa mucho tu bienestar. Necesitas ayuda inmediata. Por favor, contacta a la Universidad del Valle - Tuluá a través del correo serviciopsicologico.tulua@correounivalle.edu.co. Tu vida tiene valor. Por favor, contacta estos recursos AHORA. No estás solo/a.</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>sadness</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1793,6 +1943,16 @@
           <t>anger</t>
         </is>
       </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>Entiendo que te sientas así, a veces el semestre puede ser abrumador. ¿Qué tal si te tomas un momento para respirar y pensar en pequeños pasos que puedas dar? Tal vez podrías hacer una lista de las cosas que te están estresando y ver si hay alguna manera de manejarlas una a una. Recuerda que está bien pedir ayuda si la necesitas. ¡Tú puedes con esto!</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>anger</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1872,6 +2032,16 @@
         </is>
       </c>
       <c r="R17" t="inlineStr">
+        <is>
+          <t>others</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>Las discusiones en grupos pueden ser realmente difíciles. Lo primero que podrías hacer es tomarte un momento para calmarte y reflexionar sobre lo que sucedió. Luego, intenta hablar con tus compañeros de manera abierta y honesta. A veces, expresar cómo te sientes y escuchar a los demás puede ayudar a encontrar un terreno común. Recuerda que todos están ahí para aprender y trabajar juntos. ¡Confía en que puedes resolverlo!</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
         <is>
           <t>others</t>
         </is>
@@ -1963,6 +2133,16 @@
           <t>sadness</t>
         </is>
       </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>Es completamente normal extrañar a tu familia y tu hogar, especialmente cuando estás en un lugar nuevo. La soledad puede ser difícil de manejar, pero hay formas de sentirte más conectado. Intenta programar videollamadas con tu familia o amigos, o incluso busca grupos de apoyo en la universidad donde puedas conocer a otros que se sientan igual. También podrías explorar actividades o clubes que te interesen; eso puede ayudarte a hacer nuevos amigos y sentirte más en casa. ¡No estás solo en esto!</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>sadness</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2045,6 +2225,16 @@
           <t>fear</t>
         </is>
       </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Es normal sentir esa tentación, especialmente cuando la presión es alta. Pero recuerda que copiarte no es la solución y puede traerte más problemas a largo plazo. En lugar de eso, intenta repasar lo que has estudiado y confía en tus capacidades. Si sientes que necesitas más apoyo, considera hablar con un profesor o un compañero para aclarar dudas. ¡Tú puedes hacerlo!</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>fear</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2127,6 +2317,16 @@
           <t>joy</t>
         </is>
       </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>¡Eso es genial! Terminar un proyecto a tiempo es un gran logro y es totalmente válido sentirse orgulloso de ti mismo. Celebra ese éxito, aunque sea con algo pequeño. Recuerda que cada paso cuenta y que estás avanzando en tu camino. ¿Qué tal si escribes ese logro en un lugar visible para recordarlo y motivarte en el futuro? ¡Sigue así! 🎉</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>joy</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2203,6 +2403,16 @@
         </is>
       </c>
       <c r="R21" t="inlineStr">
+        <is>
+          <t>joy</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>¡Eso es increíble! Hacer nuevos amigos es una de las mejores partes de la experiencia universitaria. Tener a alguien con quien compartir tus días puede hacer que todo sea más divertido y menos estresante. ¿Ya han hecho algo juntos o tienen planes para salir? ¡Aprovecha esa nueva amistad! 🎉</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
         <is>
           <t>joy</t>
         </is>
@@ -2247,6 +2457,16 @@
           <t>others</t>
         </is>
       </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>Parece que no has escrito nada. Si necesitas hablar de algo o tienes alguna pregunta, aquí estoy para ayudarte. ¡Cuéntame!</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>others</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>